<commit_message>
Segunda optimización de Kp
</commit_message>
<xml_diff>
--- a/Calculador Kp.xlsx
+++ b/Calculador Kp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlour\Desktop\TELECO\4º.2\SECO\E2\SECO-E2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA1C6D4-7093-4E1B-ADB2-210DD4924643}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DC0995-7F5B-4C1C-A778-9FE7243425A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12990" yWindow="1245" windowWidth="12450" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9450" yWindow="495" windowWidth="12450" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kp" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>km</t>
   </si>
@@ -69,8 +69,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -115,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -297,12 +297,47 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -311,9 +346,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -322,7 +355,7 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -335,7 +368,16 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -344,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -359,9 +401,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,79 +425,100 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -743,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,277 +817,277 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="27"/>
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
-        <v>6400.1</v>
-      </c>
-      <c r="E3" s="25">
+      <c r="C3" s="11">
+        <v>1600</v>
+      </c>
+      <c r="E3" s="19">
         <v>0.1</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="20">
         <f>C4/(2*E3)</f>
         <v>169.76999999999998</v>
       </c>
-      <c r="G3" s="27">
-        <f>EXP(-(E3/SQRT(1-(E3^2)))*PI())</f>
+      <c r="G3" s="21">
+        <f t="shared" ref="G3:G11" si="0">EXP(-(E3/SQRT(1-(E3^2)))*PI())</f>
         <v>0.72924761428767093</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="22">
         <f>LN(1/(C5*SQRT(1-(E3^2))))/(E3*F3)</f>
         <v>0.23072675816427501</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="23">
         <f>(C4^2)/(4*(E3^2)*C3)</f>
-        <v>4.5033441508726408</v>
-      </c>
-      <c r="J3" s="30">
+        <v>18.013658062499996</v>
+      </c>
+      <c r="J3" s="24">
         <f>I3*75</f>
-        <v>337.75081131544806</v>
+        <v>1351.0243546874997</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>33.954000000000001</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>0.2</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="17">
         <f>C4/(2*E4)</f>
         <v>84.884999999999991</v>
       </c>
-      <c r="G4" s="16">
-        <f>EXP(-(E4/SQRT(1-(E4^2)))*PI())</f>
+      <c r="G4" s="14">
+        <f t="shared" si="0"/>
         <v>0.52662059933030292</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="18">
         <f>LN(1/(C5*SQRT(1-(E4^2))))/(E4*F4)</f>
         <v>0.23163303308524907</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="16">
         <f>(C4^2)/(4*(E4^2)*C3)</f>
-        <v>1.1258360377181602</v>
+        <v>4.5034145156249989</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" ref="J4:J11" si="0">I4*75</f>
-        <v>84.437702828862015</v>
+        <f t="shared" ref="J4:J11" si="1">I4*75</f>
+        <v>337.75608867187492</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="4">
         <v>0.02</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>0.3</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="17">
         <f>C4/(2*E5)</f>
         <v>56.59</v>
       </c>
-      <c r="G5" s="16">
-        <f>EXP(-(E5/SQRT(1-(E5^2)))*PI())</f>
+      <c r="G5" s="14">
+        <f t="shared" si="0"/>
         <v>0.37232610492658641</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="18">
         <f>LN(1/(C5*SQRT(1-(E5^2))))/(E5*F5)</f>
         <v>0.23320836102749407</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="15">
         <f>(C4^2)/(4*(E5^2)*C3)</f>
-        <v>0.5003715723191825</v>
+        <v>2.0015175625000001</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" si="0"/>
-        <v>37.527867923938686</v>
+        <f t="shared" si="1"/>
+        <v>150.11381718750002</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>0.4</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="17">
         <f>C4/(2*E6)</f>
         <v>42.442499999999995</v>
       </c>
-      <c r="G6" s="16">
-        <f>EXP(-(E6/SQRT(1-(E6^2)))*PI())</f>
+      <c r="G6" s="14">
+        <f t="shared" si="0"/>
         <v>0.25382672198010869</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="18">
         <f>LN(1/(C5*SQRT(1-(E6^2))))/(E6*F6)</f>
         <v>0.23556574771753164</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="15">
         <f>(C4^2)/(4*(E6^2)*C3)</f>
-        <v>0.28145900942954005</v>
+        <v>1.1258536289062497</v>
       </c>
       <c r="J6" s="5">
-        <f t="shared" si="0"/>
-        <v>21.109425707215504</v>
+        <f t="shared" si="1"/>
+        <v>84.43902216796873</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>0.5</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="17">
         <f>C4/(2*E7)</f>
         <v>33.954000000000001</v>
       </c>
-      <c r="G7" s="16">
-        <f>EXP(-(E7/SQRT(1-(E7^2)))*PI())</f>
+      <c r="G7" s="14">
+        <f t="shared" si="0"/>
         <v>0.16303353482158042</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="18">
         <f>LN(1/(C5*SQRT(1-(E7^2))))/(E7*F7)</f>
         <v>0.2389034600726887</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="15">
         <f>(C4^2)/(4*(E7^2)*C3)</f>
-        <v>0.18013376603490569</v>
+        <v>0.72054632249999995</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="0"/>
-        <v>13.510032452617926</v>
+        <f t="shared" si="1"/>
+        <v>54.040974187499998</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>0.6</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="17">
         <f>C4/(2*E8)</f>
         <v>28.295000000000002</v>
       </c>
-      <c r="G8" s="16">
-        <f>EXP(-(E8/SQRT(1-(E8^2)))*PI())</f>
+      <c r="G8" s="14">
+        <f t="shared" si="0"/>
         <v>9.4780224842154898E-2</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="18">
         <f>LN(1/(C5*SQRT(1-(E8^2))))/(E8*F8)</f>
         <v>0.24357463372458951</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="16">
         <f>(C4^2)/(4*(E8^2)*C3)</f>
-        <v>0.12509289307979563</v>
+        <v>0.50037939062500003</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="0"/>
-        <v>9.3819669809846715</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>37.528454296875005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="E9" s="13">
+      <c r="E9" s="28">
         <v>0.7</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="29">
         <f>C4/(2*E9)</f>
         <v>24.252857142857145</v>
       </c>
-      <c r="G9" s="16">
-        <f>EXP(-(E9/SQRT(1-(E9^2)))*PI())</f>
+      <c r="G9" s="30">
+        <f t="shared" si="0"/>
         <v>4.5987910260267752E-2</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="31">
         <f>LN(1/(C5*SQRT(1-(E9^2))))/(E9*F9)</f>
         <v>0.25026184143606228</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="32">
         <f>(C4^2)/(4*(E9^2)*C3)</f>
-        <v>9.1904982670870258E-2</v>
-      </c>
-      <c r="J9" s="5">
-        <f t="shared" si="0"/>
-        <v>6.8928737003152696</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="34">
+        <v>0.36762567474489799</v>
+      </c>
+      <c r="J9" s="33">
+        <f t="shared" si="1"/>
+        <v>27.571925605867349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="40">
         <v>0.8</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="41">
         <f>C4/(2*E10)</f>
         <v>21.221249999999998</v>
       </c>
-      <c r="G10" s="36">
-        <f>EXP(-(E10/SQRT(1-(E10^2)))*PI())</f>
+      <c r="G10" s="42">
+        <f t="shared" si="0"/>
         <v>1.516461986454655E-2</v>
       </c>
-      <c r="H10" s="37">
+      <c r="H10" s="43">
         <f>LN(1/(C5*SQRT(1-(E10^2))))/(E10*F10)</f>
         <v>0.26052003470543306</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="44">
         <f>(C4^2)/(4*(E10^2)*C3)</f>
-        <v>7.0364752357385013E-2</v>
-      </c>
-      <c r="J10" s="39">
-        <f t="shared" si="0"/>
-        <v>5.277356426803876</v>
+        <v>0.28146340722656243</v>
+      </c>
+      <c r="J10" s="45">
+        <f t="shared" si="1"/>
+        <v>21.109755541992183</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
-      <c r="E11" s="15">
+      <c r="E11" s="34">
         <v>0.9</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="35">
         <f>C4/(2*E11)</f>
         <v>18.863333333333333</v>
       </c>
-      <c r="G11" s="17">
-        <f>EXP(-(E11/SQRT(1-(E11^2)))*PI())</f>
+      <c r="G11" s="36">
+        <f t="shared" si="0"/>
         <v>1.5237558205194084E-3</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="37">
         <f>LN(1/(C5*SQRT(1-(E11^2))))/(E11*F11)</f>
         <v>0.27934196906632336</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="38">
         <f>(C4^2)/(4*(E11^2)*C3)</f>
-        <v>5.5596841368798042E-2</v>
-      </c>
-      <c r="J11" s="6">
-        <f t="shared" si="0"/>
-        <v>4.1697631026598527</v>
+        <v>0.22239084027777778</v>
+      </c>
+      <c r="J11" s="39">
+        <f t="shared" si="1"/>
+        <v>16.679313020833334</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>